<commit_message>
late hour cutoff update
</commit_message>
<xml_diff>
--- a/output/report_project_1-30_September_2024.xlsx
+++ b/output/report_project_1-30_September_2024.xlsx
@@ -1083,127 +1083,127 @@
       </c>
       <c r="B6" s="16" t="inlineStr">
         <is>
-          <t>HERMANTO</t>
+          <t>MICERI KARDIAS DOMINI</t>
         </is>
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>STORE</t>
+          <t>WELDER T</t>
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E6" s="17" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="17" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="G6" s="17" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H6" s="17" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="I6" s="17" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="J6" s="17" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="K6" s="17" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L6" s="17" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="M6" s="17" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="N6" s="17" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="O6" s="17" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="P6" s="17" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="Q6" s="17" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="R6" s="17" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="S6" s="17" t="n">
         <v>0</v>
       </c>
       <c r="T6" s="17" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="U6" s="17" t="n">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="V6" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="W6" s="17" t="n">
         <v>8.5</v>
       </c>
-      <c r="W6" s="17" t="n">
-        <v>7</v>
-      </c>
       <c r="X6" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="Y6" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z6" s="17" t="n">
         <v>10.5</v>
       </c>
-      <c r="Y6" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="Z6" s="17" t="n">
-        <v>0</v>
-      </c>
       <c r="AA6" s="7" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="AB6" s="7" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="AC6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AD6" s="7" t="n">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="AE6" s="7" t="n">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="AF6" s="7" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AG6" s="7" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="AH6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AI6" s="18" t="n">
-        <v>45</v>
+        <v>287</v>
       </c>
       <c r="AJ6" s="19" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="AK6" s="20" t="n">
         <v>20000</v>
       </c>
       <c r="AL6" s="21" t="n">
-        <v>21000</v>
+        <v>20000</v>
       </c>
       <c r="AM6" s="22" t="n">
-        <v>100000</v>
+        <v>540000</v>
       </c>
       <c r="AN6" s="22" t="n">
-        <v>945000</v>
+        <v>5740000</v>
       </c>
       <c r="AO6" s="23" t="n">
-        <v>1045000</v>
+        <v>6280000</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="39">

</xml_diff>

<commit_message>
add report gaji harian
</commit_message>
<xml_diff>
--- a/output/report_project_1-30_September_2024.xlsx
+++ b/output/report_project_1-30_September_2024.xlsx
@@ -1095,7 +1095,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="17" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="F6" s="17" t="n">
         <v>10.5</v>
@@ -1104,7 +1104,7 @@
         <v>2.5</v>
       </c>
       <c r="H6" s="17" t="n">
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="I6" s="17" t="n">
         <v>8.5</v>
@@ -1119,7 +1119,7 @@
         <v>10.5</v>
       </c>
       <c r="M6" s="17" t="n">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="N6" s="17" t="n">
         <v>10.5</v>
@@ -1137,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="S6" s="17" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="T6" s="17" t="n">
         <v>10.5</v>
@@ -1167,7 +1167,7 @@
         <v>10.5</v>
       </c>
       <c r="AC6" s="7" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="AD6" s="7" t="n">
         <v>11.5</v>
@@ -1185,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="AI6" s="18" t="n">
-        <v>287</v>
+        <v>287.5</v>
       </c>
       <c r="AJ6" s="19" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AK6" s="20" t="n">
         <v>20000</v>
@@ -1197,374 +1197,1046 @@
         <v>20000</v>
       </c>
       <c r="AM6" s="22" t="n">
-        <v>540000</v>
+        <v>520000</v>
       </c>
       <c r="AN6" s="22" t="n">
-        <v>5740000</v>
+        <v>5750000</v>
       </c>
       <c r="AO6" s="23" t="n">
-        <v>6280000</v>
+        <v>6270000</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="39">
       <c r="A7" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="16" t="n"/>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="17" t="n"/>
-      <c r="F7" s="17" t="n"/>
-      <c r="G7" s="17" t="n"/>
-      <c r="H7" s="17" t="n"/>
-      <c r="I7" s="17" t="n"/>
-      <c r="J7" s="17" t="n"/>
-      <c r="K7" s="17" t="n"/>
-      <c r="L7" s="17" t="n"/>
-      <c r="M7" s="17" t="n"/>
-      <c r="N7" s="17" t="n"/>
-      <c r="O7" s="17" t="n"/>
-      <c r="P7" s="17" t="n"/>
-      <c r="Q7" s="17" t="n"/>
-      <c r="R7" s="17" t="n"/>
-      <c r="S7" s="17" t="n"/>
-      <c r="T7" s="17" t="n"/>
-      <c r="U7" s="17" t="n"/>
-      <c r="V7" s="17" t="n"/>
-      <c r="W7" s="17" t="n"/>
-      <c r="X7" s="17" t="n"/>
-      <c r="Y7" s="17" t="n"/>
-      <c r="Z7" s="17" t="n"/>
-      <c r="AA7" s="7" t="n"/>
-      <c r="AB7" s="7" t="n"/>
-      <c r="AC7" s="7" t="n"/>
-      <c r="AD7" s="7" t="n"/>
-      <c r="AE7" s="7" t="n"/>
-      <c r="AF7" s="7" t="n"/>
-      <c r="AG7" s="7" t="n"/>
-      <c r="AH7" s="7" t="n"/>
-      <c r="AI7" s="18" t="n"/>
-      <c r="AJ7" s="19" t="n"/>
-      <c r="AK7" s="20" t="n"/>
-      <c r="AL7" s="21" t="n"/>
-      <c r="AM7" s="22" t="n"/>
-      <c r="AN7" s="22" t="n"/>
-      <c r="AO7" s="23" t="n"/>
+      <c r="B7" s="16" t="inlineStr">
+        <is>
+          <t>PUTRA ANTONIUS MANALU</t>
+        </is>
+      </c>
+      <c r="C7" s="16" t="inlineStr">
+        <is>
+          <t>FITTER</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="E7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="F7" s="17" t="n">
+        <v/>
+      </c>
+      <c r="G7" s="17" t="n">
+        <v/>
+      </c>
+      <c r="H7" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I7" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="J7" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="K7" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="L7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="M7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="O7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="P7" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="Q7" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="R7" s="17" t="n">
+        <v>9</v>
+      </c>
+      <c r="S7" s="17" t="n">
+        <v/>
+      </c>
+      <c r="T7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="U7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="V7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="W7" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="X7" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="Y7" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z7" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AA7" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AB7" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AC7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AE7" s="7" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="AF7" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG7" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AH7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="18" t="n">
+        <v>266.5</v>
+      </c>
+      <c r="AJ7" s="19" t="n">
+        <v>24</v>
+      </c>
+      <c r="AK7" s="20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL7" s="21" t="n">
+        <v>22000</v>
+      </c>
+      <c r="AM7" s="22" t="n">
+        <v>480000</v>
+      </c>
+      <c r="AN7" s="22" t="n">
+        <v>5863000</v>
+      </c>
+      <c r="AO7" s="23" t="n">
+        <v>6343000</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="39">
       <c r="A8" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="16" t="n"/>
-      <c r="C8" s="16" t="n"/>
-      <c r="D8" s="7" t="n"/>
-      <c r="E8" s="17" t="n"/>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
-      <c r="H8" s="17" t="n"/>
-      <c r="I8" s="17" t="n"/>
-      <c r="J8" s="17" t="n"/>
-      <c r="K8" s="17" t="n"/>
-      <c r="L8" s="17" t="n"/>
-      <c r="M8" s="17" t="n"/>
-      <c r="N8" s="17" t="n"/>
-      <c r="O8" s="17" t="n"/>
-      <c r="P8" s="17" t="n"/>
-      <c r="Q8" s="17" t="n"/>
-      <c r="R8" s="17" t="n"/>
-      <c r="S8" s="17" t="n"/>
-      <c r="T8" s="17" t="n"/>
-      <c r="U8" s="17" t="n"/>
-      <c r="V8" s="17" t="n"/>
-      <c r="W8" s="17" t="n"/>
-      <c r="X8" s="17" t="n"/>
-      <c r="Y8" s="17" t="n"/>
-      <c r="Z8" s="17" t="n"/>
-      <c r="AA8" s="7" t="n"/>
-      <c r="AB8" s="7" t="n"/>
-      <c r="AC8" s="7" t="n"/>
-      <c r="AD8" s="7" t="n"/>
-      <c r="AE8" s="7" t="n"/>
-      <c r="AF8" s="7" t="n"/>
-      <c r="AG8" s="7" t="n"/>
-      <c r="AH8" s="7" t="n"/>
-      <c r="AI8" s="18" t="n"/>
-      <c r="AJ8" s="19" t="n"/>
-      <c r="AK8" s="20" t="n"/>
-      <c r="AL8" s="21" t="n"/>
-      <c r="AM8" s="22" t="n"/>
-      <c r="AN8" s="22" t="n"/>
-      <c r="AO8" s="23" t="n"/>
+      <c r="B8" s="16" t="inlineStr">
+        <is>
+          <t>BENI ELMON PARDEDE</t>
+        </is>
+      </c>
+      <c r="C8" s="16" t="inlineStr">
+        <is>
+          <t>FITTER</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="E8" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="F8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="G8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="H8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I8" s="17" t="n">
+        <v>456</v>
+      </c>
+      <c r="J8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="K8" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="L8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="M8" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="N8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="O8" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="P8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="Q8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="R8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="S8" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="T8" s="17" t="n">
+        <v>392</v>
+      </c>
+      <c r="U8" s="17" t="n">
+        <v>328</v>
+      </c>
+      <c r="V8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="W8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="X8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="Y8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="Z8" s="17" t="n">
+        <v/>
+      </c>
+      <c r="AA8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AB8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AC8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AD8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AE8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AF8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AG8" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AH8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="18" t="n">
+        <v>4080</v>
+      </c>
+      <c r="AJ8" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK8" s="20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL8" s="21" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AM8" s="22" t="n">
+        <v>160000</v>
+      </c>
+      <c r="AN8" s="22" t="n">
+        <v>81600000</v>
+      </c>
+      <c r="AO8" s="23" t="n">
+        <v>81760000</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="39">
       <c r="A9" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="16" t="n"/>
-      <c r="C9" s="16" t="n"/>
-      <c r="D9" s="7" t="n"/>
-      <c r="E9" s="17" t="n"/>
-      <c r="F9" s="17" t="n"/>
-      <c r="G9" s="17" t="n"/>
-      <c r="H9" s="17" t="n"/>
-      <c r="I9" s="17" t="n"/>
-      <c r="J9" s="17" t="n"/>
-      <c r="K9" s="17" t="n"/>
-      <c r="L9" s="17" t="n"/>
-      <c r="M9" s="17" t="n"/>
-      <c r="N9" s="17" t="n"/>
-      <c r="O9" s="17" t="n"/>
-      <c r="P9" s="17" t="n"/>
-      <c r="Q9" s="17" t="n"/>
-      <c r="R9" s="17" t="n"/>
-      <c r="S9" s="17" t="n"/>
-      <c r="T9" s="17" t="n"/>
-      <c r="U9" s="17" t="n"/>
-      <c r="V9" s="17" t="n"/>
-      <c r="W9" s="17" t="n"/>
-      <c r="X9" s="17" t="n"/>
-      <c r="Y9" s="17" t="n"/>
-      <c r="Z9" s="17" t="n"/>
-      <c r="AA9" s="7" t="n"/>
-      <c r="AB9" s="7" t="n"/>
-      <c r="AC9" s="7" t="n"/>
-      <c r="AD9" s="7" t="n"/>
-      <c r="AE9" s="7" t="n"/>
-      <c r="AF9" s="7" t="n"/>
-      <c r="AG9" s="7" t="n"/>
-      <c r="AH9" s="7" t="n"/>
-      <c r="AI9" s="18" t="n"/>
-      <c r="AJ9" s="19" t="n"/>
-      <c r="AK9" s="20" t="n"/>
-      <c r="AL9" s="21" t="n"/>
-      <c r="AM9" s="22" t="n"/>
-      <c r="AN9" s="22" t="n"/>
-      <c r="AO9" s="23" t="n"/>
+      <c r="B9" s="16" t="inlineStr">
+        <is>
+          <t>PONIMIN SIBANGEBANGE</t>
+        </is>
+      </c>
+      <c r="C9" s="16" t="inlineStr">
+        <is>
+          <t>WELDER</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="E9" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="F9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="G9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="H9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I9" s="17" t="n">
+        <v>456</v>
+      </c>
+      <c r="J9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="K9" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="L9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="M9" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="N9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="O9" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="P9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="Q9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="R9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="S9" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="T9" s="17" t="n">
+        <v>392</v>
+      </c>
+      <c r="U9" s="17" t="n">
+        <v>328</v>
+      </c>
+      <c r="V9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="W9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="X9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="Y9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="Z9" s="17" t="n">
+        <v/>
+      </c>
+      <c r="AA9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AB9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AC9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AD9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AE9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AF9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AG9" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AH9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="18" t="n">
+        <v>4080</v>
+      </c>
+      <c r="AJ9" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK9" s="20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL9" s="21" t="n">
+        <v>22000</v>
+      </c>
+      <c r="AM9" s="22" t="n">
+        <v>160000</v>
+      </c>
+      <c r="AN9" s="22" t="n">
+        <v>89760000</v>
+      </c>
+      <c r="AO9" s="23" t="n">
+        <v>89920000</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="39">
       <c r="A10" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="16" t="n"/>
-      <c r="C10" s="16" t="n"/>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="17" t="n"/>
-      <c r="F10" s="17" t="n"/>
-      <c r="G10" s="17" t="n"/>
-      <c r="H10" s="17" t="n"/>
-      <c r="I10" s="17" t="n"/>
-      <c r="J10" s="17" t="n"/>
-      <c r="K10" s="17" t="n"/>
-      <c r="L10" s="17" t="n"/>
-      <c r="M10" s="17" t="n"/>
-      <c r="N10" s="17" t="n"/>
-      <c r="O10" s="17" t="n"/>
-      <c r="P10" s="17" t="n"/>
-      <c r="Q10" s="17" t="n"/>
-      <c r="R10" s="17" t="n"/>
-      <c r="S10" s="17" t="n"/>
-      <c r="T10" s="17" t="n"/>
-      <c r="U10" s="17" t="n"/>
-      <c r="V10" s="17" t="n"/>
-      <c r="W10" s="17" t="n"/>
-      <c r="X10" s="17" t="n"/>
-      <c r="Y10" s="17" t="n"/>
-      <c r="Z10" s="17" t="n"/>
-      <c r="AA10" s="7" t="n"/>
-      <c r="AB10" s="7" t="n"/>
-      <c r="AC10" s="7" t="n"/>
-      <c r="AD10" s="7" t="n"/>
-      <c r="AE10" s="7" t="n"/>
-      <c r="AF10" s="7" t="n"/>
-      <c r="AG10" s="7" t="n"/>
-      <c r="AH10" s="7" t="n"/>
-      <c r="AI10" s="18" t="n"/>
-      <c r="AJ10" s="19" t="n"/>
-      <c r="AK10" s="20" t="n"/>
-      <c r="AL10" s="21" t="n"/>
-      <c r="AM10" s="22" t="n"/>
-      <c r="AN10" s="22" t="n"/>
-      <c r="AO10" s="23" t="n"/>
+      <c r="B10" s="16" t="inlineStr">
+        <is>
+          <t>MURDIONO SITINJAK</t>
+        </is>
+      </c>
+      <c r="C10" s="16" t="inlineStr">
+        <is>
+          <t>WELDER</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v/>
+      </c>
+      <c r="E10" s="17" t="n">
+        <v/>
+      </c>
+      <c r="F10" s="17" t="n">
+        <v>296</v>
+      </c>
+      <c r="G10" s="17" t="n">
+        <v/>
+      </c>
+      <c r="H10" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I10" s="17" t="n">
+        <v/>
+      </c>
+      <c r="J10" s="17" t="n">
+        <v>520</v>
+      </c>
+      <c r="K10" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="L10" s="17" t="n">
+        <v/>
+      </c>
+      <c r="M10" s="17" t="n">
+        <v/>
+      </c>
+      <c r="N10" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="O10" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="P10" s="17" t="n">
+        <v>456</v>
+      </c>
+      <c r="Q10" s="17" t="n">
+        <v>520</v>
+      </c>
+      <c r="R10" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="S10" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="T10" s="17" t="n">
+        <v/>
+      </c>
+      <c r="U10" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="V10" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="W10" s="17" t="n">
+        <v>456</v>
+      </c>
+      <c r="X10" s="17" t="n">
+        <v>424</v>
+      </c>
+      <c r="Y10" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="Z10" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="AA10" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AB10" s="7" t="n">
+        <v>488</v>
+      </c>
+      <c r="AC10" s="7" t="n">
+        <v>360</v>
+      </c>
+      <c r="AD10" s="7" t="n">
+        <v>552</v>
+      </c>
+      <c r="AE10" s="7" t="n">
+        <v>488</v>
+      </c>
+      <c r="AF10" s="7" t="n">
+        <v>720</v>
+      </c>
+      <c r="AG10" s="7" t="n">
+        <v>488</v>
+      </c>
+      <c r="AH10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="18" t="n">
+        <v>11088</v>
+      </c>
+      <c r="AJ10" s="19" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK10" s="20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL10" s="21" t="n">
+        <v>22000</v>
+      </c>
+      <c r="AM10" s="22" t="n">
+        <v>420000</v>
+      </c>
+      <c r="AN10" s="22" t="n">
+        <v>243936000</v>
+      </c>
+      <c r="AO10" s="23" t="n">
+        <v>244356000</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="39">
       <c r="A11" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="16" t="n"/>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="17" t="n"/>
-      <c r="F11" s="17" t="n"/>
-      <c r="G11" s="17" t="n"/>
-      <c r="H11" s="17" t="n"/>
-      <c r="I11" s="17" t="n"/>
-      <c r="J11" s="17" t="n"/>
-      <c r="K11" s="17" t="n"/>
-      <c r="L11" s="17" t="n"/>
-      <c r="M11" s="17" t="n"/>
-      <c r="N11" s="17" t="n"/>
-      <c r="O11" s="17" t="n"/>
-      <c r="P11" s="17" t="n"/>
-      <c r="Q11" s="17" t="n"/>
-      <c r="R11" s="17" t="n"/>
-      <c r="S11" s="17" t="n"/>
-      <c r="T11" s="17" t="n"/>
-      <c r="U11" s="17" t="n"/>
-      <c r="V11" s="17" t="n"/>
-      <c r="W11" s="17" t="n"/>
-      <c r="X11" s="17" t="n"/>
-      <c r="Y11" s="17" t="n"/>
-      <c r="Z11" s="17" t="n"/>
-      <c r="AA11" s="7" t="n"/>
-      <c r="AB11" s="7" t="n"/>
-      <c r="AC11" s="7" t="n"/>
-      <c r="AD11" s="7" t="n"/>
-      <c r="AE11" s="7" t="n"/>
-      <c r="AF11" s="7" t="n"/>
-      <c r="AG11" s="7" t="n"/>
-      <c r="AH11" s="7" t="n"/>
-      <c r="AI11" s="18" t="n"/>
-      <c r="AJ11" s="19" t="n"/>
-      <c r="AK11" s="20" t="n"/>
-      <c r="AL11" s="21" t="n"/>
-      <c r="AM11" s="22" t="n"/>
-      <c r="AN11" s="22" t="n"/>
-      <c r="AO11" s="23" t="n"/>
+      <c r="B11" s="16" t="inlineStr">
+        <is>
+          <t>PRENGKI SIHOMBING</t>
+        </is>
+      </c>
+      <c r="C11" s="16" t="inlineStr">
+        <is>
+          <t>FITTER</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v/>
+      </c>
+      <c r="E11" s="17" t="n">
+        <v/>
+      </c>
+      <c r="F11" s="17" t="n">
+        <v>296</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v/>
+      </c>
+      <c r="H11" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I11" s="17" t="n">
+        <v/>
+      </c>
+      <c r="J11" s="17" t="n">
+        <v>520</v>
+      </c>
+      <c r="K11" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="L11" s="17" t="n">
+        <v/>
+      </c>
+      <c r="M11" s="17" t="n">
+        <v/>
+      </c>
+      <c r="N11" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="O11" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="P11" s="17" t="n">
+        <v>456</v>
+      </c>
+      <c r="Q11" s="17" t="n">
+        <v>520</v>
+      </c>
+      <c r="R11" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="S11" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="T11" s="17" t="n">
+        <v/>
+      </c>
+      <c r="U11" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="V11" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="W11" s="17" t="n">
+        <v>456</v>
+      </c>
+      <c r="X11" s="17" t="n">
+        <v>424</v>
+      </c>
+      <c r="Y11" s="17" t="n">
+        <v>720</v>
+      </c>
+      <c r="Z11" s="17" t="n">
+        <v>488</v>
+      </c>
+      <c r="AA11" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AB11" s="7" t="n">
+        <v>488</v>
+      </c>
+      <c r="AC11" s="7" t="n">
+        <v>360</v>
+      </c>
+      <c r="AD11" s="7" t="n">
+        <v>552</v>
+      </c>
+      <c r="AE11" s="7" t="n">
+        <v>488</v>
+      </c>
+      <c r="AF11" s="7" t="n">
+        <v>720</v>
+      </c>
+      <c r="AG11" s="7" t="n">
+        <v>488</v>
+      </c>
+      <c r="AH11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="18" t="n">
+        <v>11088</v>
+      </c>
+      <c r="AJ11" s="19" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK11" s="20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL11" s="21" t="n">
+        <v>22500</v>
+      </c>
+      <c r="AM11" s="22" t="n">
+        <v>420000</v>
+      </c>
+      <c r="AN11" s="22" t="n">
+        <v>249480000</v>
+      </c>
+      <c r="AO11" s="23" t="n">
+        <v>249900000</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="39">
       <c r="A12" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="16" t="n"/>
-      <c r="C12" s="16" t="n"/>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="17" t="n"/>
-      <c r="F12" s="17" t="n"/>
-      <c r="G12" s="17" t="n"/>
-      <c r="H12" s="17" t="n"/>
-      <c r="I12" s="17" t="n"/>
-      <c r="J12" s="17" t="n"/>
-      <c r="K12" s="17" t="n"/>
-      <c r="L12" s="17" t="n"/>
-      <c r="M12" s="17" t="n"/>
-      <c r="N12" s="17" t="n"/>
-      <c r="O12" s="17" t="n"/>
-      <c r="P12" s="17" t="n"/>
-      <c r="Q12" s="17" t="n"/>
-      <c r="R12" s="17" t="n"/>
-      <c r="S12" s="17" t="n"/>
-      <c r="T12" s="17" t="n"/>
-      <c r="U12" s="17" t="n"/>
-      <c r="V12" s="17" t="n"/>
-      <c r="W12" s="17" t="n"/>
-      <c r="X12" s="17" t="n"/>
-      <c r="Y12" s="17" t="n"/>
-      <c r="Z12" s="17" t="n"/>
-      <c r="AA12" s="7" t="n"/>
-      <c r="AB12" s="7" t="n"/>
-      <c r="AC12" s="7" t="n"/>
-      <c r="AD12" s="7" t="n"/>
-      <c r="AE12" s="7" t="n"/>
-      <c r="AF12" s="7" t="n"/>
-      <c r="AG12" s="7" t="n"/>
-      <c r="AH12" s="7" t="n"/>
-      <c r="AI12" s="18" t="n"/>
-      <c r="AJ12" s="19" t="n"/>
-      <c r="AK12" s="20" t="n"/>
-      <c r="AL12" s="21" t="n"/>
-      <c r="AM12" s="22" t="n"/>
-      <c r="AN12" s="22" t="n"/>
-      <c r="AO12" s="23" t="n"/>
+      <c r="B12" s="16" t="inlineStr">
+        <is>
+          <t>HALLASON SINAMBELA</t>
+        </is>
+      </c>
+      <c r="C12" s="16" t="inlineStr">
+        <is>
+          <t>FOREMAN WELDER</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v/>
+      </c>
+      <c r="E12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="F12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G12" s="17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H12" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I12" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="J12" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="K12" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="L12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="M12" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="N12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="O12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="P12" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="Q12" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="R12" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="S12" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="T12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="U12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="V12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="W12" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="X12" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="Y12" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z12" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AA12" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AB12" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AC12" s="7" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AD12" s="7" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="AE12" s="7" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="AF12" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AG12" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AH12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="18" t="n">
+        <v>273.5</v>
+      </c>
+      <c r="AJ12" s="19" t="n">
+        <v>25</v>
+      </c>
+      <c r="AK12" s="20" t="n">
+        <v>25000</v>
+      </c>
+      <c r="AL12" s="21" t="n">
+        <v>27000</v>
+      </c>
+      <c r="AM12" s="22" t="n">
+        <v>625000</v>
+      </c>
+      <c r="AN12" s="22" t="n">
+        <v>7384500</v>
+      </c>
+      <c r="AO12" s="23" t="n">
+        <v>8009500</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="39">
       <c r="A13" s="15" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="16" t="n"/>
-      <c r="C13" s="16" t="n"/>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="17" t="n"/>
-      <c r="F13" s="17" t="n"/>
-      <c r="G13" s="17" t="n"/>
-      <c r="H13" s="17" t="n"/>
-      <c r="I13" s="17" t="n"/>
-      <c r="J13" s="17" t="n"/>
-      <c r="K13" s="17" t="n"/>
-      <c r="L13" s="17" t="n"/>
-      <c r="M13" s="17" t="n"/>
-      <c r="N13" s="17" t="n"/>
-      <c r="O13" s="17" t="n"/>
-      <c r="P13" s="17" t="n"/>
-      <c r="Q13" s="17" t="n"/>
-      <c r="R13" s="17" t="n"/>
-      <c r="S13" s="17" t="n"/>
-      <c r="T13" s="17" t="n"/>
-      <c r="U13" s="17" t="n"/>
-      <c r="V13" s="17" t="n"/>
-      <c r="W13" s="17" t="n"/>
-      <c r="X13" s="17" t="n"/>
-      <c r="Y13" s="17" t="n"/>
-      <c r="Z13" s="17" t="n"/>
-      <c r="AA13" s="7" t="n"/>
-      <c r="AB13" s="7" t="n"/>
-      <c r="AC13" s="7" t="n"/>
-      <c r="AD13" s="7" t="n"/>
-      <c r="AE13" s="7" t="n"/>
-      <c r="AF13" s="7" t="n"/>
-      <c r="AG13" s="7" t="n"/>
-      <c r="AH13" s="7" t="n"/>
-      <c r="AI13" s="18" t="n"/>
-      <c r="AJ13" s="19" t="n"/>
-      <c r="AK13" s="20" t="n"/>
-      <c r="AL13" s="21" t="n"/>
-      <c r="AM13" s="22" t="n"/>
-      <c r="AN13" s="22" t="n"/>
-      <c r="AO13" s="23" t="n"/>
+      <c r="B13" s="16" t="inlineStr">
+        <is>
+          <t>MUHAMMAD ABDUL ISNAN</t>
+        </is>
+      </c>
+      <c r="C13" s="16" t="inlineStr">
+        <is>
+          <t>WELDER</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="E13" s="17" t="n">
+        <v/>
+      </c>
+      <c r="F13" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G13" s="17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H13" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I13" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="J13" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="K13" s="17" t="n">
+        <v/>
+      </c>
+      <c r="L13" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="M13" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="N13" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="O13" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="P13" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="Q13" s="17" t="n">
+        <v/>
+      </c>
+      <c r="R13" s="17" t="n">
+        <v/>
+      </c>
+      <c r="S13" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="T13" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="U13" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="V13" s="17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="W13" s="17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="X13" s="17" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="Y13" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z13" s="17" t="n">
+        <v/>
+      </c>
+      <c r="AA13" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AB13" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AC13" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AD13" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE13" s="7" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="AF13" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AG13" s="7" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="AH13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="18" t="n">
+        <v>210</v>
+      </c>
+      <c r="AJ13" s="19" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK13" s="20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL13" s="21" t="n">
+        <v>22000</v>
+      </c>
+      <c r="AM13" s="22" t="n">
+        <v>420000</v>
+      </c>
+      <c r="AN13" s="22" t="n">
+        <v>4620000</v>
+      </c>
+      <c r="AO13" s="23" t="n">
+        <v>5040000</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="39">
       <c r="A14" s="15" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="16" t="n"/>
-      <c r="C14" s="16" t="n"/>
-      <c r="D14" s="7" t="n"/>
-      <c r="E14" s="17" t="n"/>
-      <c r="F14" s="17" t="n"/>
-      <c r="G14" s="17" t="n"/>
-      <c r="H14" s="17" t="n"/>
-      <c r="I14" s="17" t="n"/>
-      <c r="J14" s="17" t="n"/>
-      <c r="K14" s="17" t="n"/>
-      <c r="L14" s="17" t="n"/>
-      <c r="M14" s="17" t="n"/>
-      <c r="N14" s="17" t="n"/>
-      <c r="O14" s="17" t="n"/>
-      <c r="P14" s="17" t="n"/>
-      <c r="Q14" s="17" t="n"/>
-      <c r="R14" s="17" t="n"/>
-      <c r="S14" s="17" t="n"/>
-      <c r="T14" s="17" t="n"/>
-      <c r="U14" s="17" t="n"/>
-      <c r="V14" s="17" t="n"/>
-      <c r="W14" s="17" t="n"/>
-      <c r="X14" s="17" t="n"/>
-      <c r="Y14" s="17" t="n"/>
-      <c r="Z14" s="17" t="n"/>
-      <c r="AA14" s="7" t="n"/>
-      <c r="AB14" s="7" t="n"/>
-      <c r="AC14" s="7" t="n"/>
-      <c r="AD14" s="7" t="n"/>
-      <c r="AE14" s="7" t="n"/>
-      <c r="AF14" s="7" t="n"/>
-      <c r="AG14" s="7" t="n"/>
-      <c r="AH14" s="7" t="n"/>
-      <c r="AI14" s="18" t="n"/>
-      <c r="AJ14" s="19" t="n"/>
-      <c r="AK14" s="20" t="n"/>
-      <c r="AL14" s="21" t="n"/>
-      <c r="AM14" s="22" t="n"/>
-      <c r="AN14" s="22" t="n"/>
-      <c r="AO14" s="23" t="n"/>
+      <c r="B14" s="16" t="inlineStr">
+        <is>
+          <t>ROYALDI HUTABARAT</t>
+        </is>
+      </c>
+      <c r="C14" s="16" t="inlineStr">
+        <is>
+          <t>HELPER</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v/>
+      </c>
+      <c r="E14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="F14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="G14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="H14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="I14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="J14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="K14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="L14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="M14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="N14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="O14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="P14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="Q14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="R14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="S14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="T14" s="17" t="n">
+        <v/>
+      </c>
+      <c r="U14" s="17" t="n">
+        <v>29</v>
+      </c>
+      <c r="V14" s="17" t="n">
+        <v>138</v>
+      </c>
+      <c r="W14" s="17" t="n">
+        <v>136</v>
+      </c>
+      <c r="X14" s="17" t="n">
+        <v>200</v>
+      </c>
+      <c r="Y14" s="17" t="n">
+        <v>56</v>
+      </c>
+      <c r="Z14" s="17" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA14" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB14" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="AC14" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AD14" s="7" t="n">
+        <v>46</v>
+      </c>
+      <c r="AE14" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="AF14" s="7" t="n">
+        <v/>
+      </c>
+      <c r="AG14" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="AH14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="18" t="n">
+        <v>823</v>
+      </c>
+      <c r="AJ14" s="19" t="n">
+        <v>11</v>
+      </c>
+      <c r="AK14" s="20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL14" s="21" t="n">
+        <v>17500</v>
+      </c>
+      <c r="AM14" s="22" t="n">
+        <v>220000</v>
+      </c>
+      <c r="AN14" s="22" t="n">
+        <v>14402500</v>
+      </c>
+      <c r="AO14" s="23" t="n">
+        <v>14622500</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="39">
       <c r="A15" s="15" t="n">

</xml_diff>